<commit_message>
Commit at 2025-04-18 14:06:14
</commit_message>
<xml_diff>
--- a/kinoco/source/data/250415/group1/1班の熱電対と試料番号の対応.xlsx
+++ b/kinoco/source/data/250415/group1/1班の熱電対と試料番号の対応.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hw/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enoki/RISME Dropbox/kinoco/Codes/01_class/lesson/kinoco/kinoco/source/data/250415/group1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CB20820-66A8-7E4B-98B2-AD5CAF311E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF950DB-674D-2245-9A85-8FAEE69CD194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{A85D305F-CD46-2441-A815-F184B894841F}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>